<commit_message>
Profile info and logout
</commit_message>
<xml_diff>
--- a/com.Equarz.Ecommerce/src/main/java/com/testdata/Registration data.xlsx
+++ b/com.Equarz.Ecommerce/src/main/java/com/testdata/Registration data.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9024"/>
+    <workbookView windowWidth="22188" windowHeight="9024" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Address" sheetId="2" r:id="rId2"/>
     <sheet name="EditAddress" sheetId="3" r:id="rId3"/>
+    <sheet name="Profile" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <r>
       <rPr>
@@ -118,6 +119,30 @@
   </si>
   <si>
     <t>main bazar,vinukonda</t>
+  </si>
+  <si>
+    <t>first name</t>
+  </si>
+  <si>
+    <t>last name</t>
+  </si>
+  <si>
+    <t>phonenumber</t>
+  </si>
+  <si>
+    <t>newpassword</t>
+  </si>
+  <si>
+    <t>confirmpassword</t>
+  </si>
+  <si>
+    <t>Niharika</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>k</t>
   </si>
 </sst>
 </file>
@@ -130,10 +155,18 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -607,140 +640,141 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1062,7 +1096,7 @@
   <sheetPr/>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -1077,22 +1111,22 @@
   </cols>
   <sheetData>
     <row r="1" ht="17.4" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1103,16 +1137,16 @@
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D2">
         <v>9515990525</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1276,4 +1310,62 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2">
+        <v>123456789</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>12345678</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>